<commit_message>
commit ors and rfq
</commit_message>
<xml_diff>
--- a/library/export_ors.xlsx
+++ b/library/export_ors.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\fas2020\library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp2\htdocs\fas2020\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9660" windowHeight="5490"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28755" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="ORS" sheetId="1" r:id="rId1"/>
@@ -754,7 +754,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="206">
+  <cellXfs count="209">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -895,18 +895,309 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="22" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="26" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -943,15 +1234,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -991,287 +1273,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="26" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="22" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1752,8 +1761,8 @@
   </sheetPr>
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+    <sheetView tabSelected="1" showRuler="0" view="pageBreakPreview" topLeftCell="A28" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56:D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2668,10 +2677,10 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="80" t="s">
+      <c r="L1" s="180" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="80"/>
+      <c r="M1" s="180"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -2685,529 +2694,529 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="99"/>
-      <c r="M2" s="99"/>
+      <c r="L2" s="193"/>
+      <c r="M2" s="193"/>
     </row>
     <row r="3" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="103" t="s">
+      <c r="A3" s="197" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="104"/>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="105"/>
-      <c r="K3" s="149" t="s">
+      <c r="B3" s="198"/>
+      <c r="C3" s="198"/>
+      <c r="D3" s="198"/>
+      <c r="E3" s="198"/>
+      <c r="F3" s="198"/>
+      <c r="G3" s="198"/>
+      <c r="H3" s="198"/>
+      <c r="I3" s="198"/>
+      <c r="J3" s="199"/>
+      <c r="K3" s="131" t="s">
         <v>41</v>
       </c>
-      <c r="L3" s="150"/>
-      <c r="M3" s="151"/>
+      <c r="L3" s="132"/>
+      <c r="M3" s="133"/>
     </row>
     <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="100" t="s">
+      <c r="A4" s="194" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="101"/>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="101"/>
-      <c r="J4" s="102"/>
-      <c r="K4" s="106" t="s">
+      <c r="B4" s="195"/>
+      <c r="C4" s="195"/>
+      <c r="D4" s="195"/>
+      <c r="E4" s="195"/>
+      <c r="F4" s="195"/>
+      <c r="G4" s="195"/>
+      <c r="H4" s="195"/>
+      <c r="I4" s="195"/>
+      <c r="J4" s="196"/>
+      <c r="K4" s="200" t="s">
         <v>43</v>
       </c>
-      <c r="L4" s="107"/>
-      <c r="M4" s="108"/>
+      <c r="L4" s="201"/>
+      <c r="M4" s="202"/>
     </row>
     <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="109" t="s">
+      <c r="A5" s="203" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="110"/>
-      <c r="C5" s="110"/>
-      <c r="D5" s="110"/>
-      <c r="E5" s="110"/>
-      <c r="F5" s="110"/>
-      <c r="G5" s="110"/>
-      <c r="H5" s="110"/>
-      <c r="I5" s="110"/>
-      <c r="J5" s="111"/>
-      <c r="K5" s="116" t="s">
+      <c r="B5" s="204"/>
+      <c r="C5" s="204"/>
+      <c r="D5" s="204"/>
+      <c r="E5" s="204"/>
+      <c r="F5" s="204"/>
+      <c r="G5" s="204"/>
+      <c r="H5" s="204"/>
+      <c r="I5" s="204"/>
+      <c r="J5" s="205"/>
+      <c r="K5" s="162" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="117"/>
-      <c r="M5" s="118"/>
+      <c r="L5" s="163"/>
+      <c r="M5" s="164"/>
     </row>
     <row r="6" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="81" t="s">
+      <c r="A6" s="137" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="82"/>
-      <c r="C6" s="83"/>
-      <c r="D6" s="87" t="s">
+      <c r="B6" s="138"/>
+      <c r="C6" s="139"/>
+      <c r="D6" s="184" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="88"/>
-      <c r="H6" s="88"/>
-      <c r="I6" s="88"/>
-      <c r="J6" s="88"/>
-      <c r="K6" s="88"/>
-      <c r="L6" s="88"/>
-      <c r="M6" s="89"/>
+      <c r="E6" s="185"/>
+      <c r="F6" s="185"/>
+      <c r="G6" s="185"/>
+      <c r="H6" s="185"/>
+      <c r="I6" s="185"/>
+      <c r="J6" s="185"/>
+      <c r="K6" s="185"/>
+      <c r="L6" s="185"/>
+      <c r="M6" s="186"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="84"/>
-      <c r="B7" s="85"/>
-      <c r="C7" s="86"/>
-      <c r="D7" s="90"/>
-      <c r="E7" s="91"/>
-      <c r="F7" s="91"/>
-      <c r="G7" s="91"/>
-      <c r="H7" s="91"/>
-      <c r="I7" s="91"/>
-      <c r="J7" s="91"/>
-      <c r="K7" s="91"/>
-      <c r="L7" s="91"/>
-      <c r="M7" s="92"/>
+      <c r="A7" s="181"/>
+      <c r="B7" s="182"/>
+      <c r="C7" s="183"/>
+      <c r="D7" s="187"/>
+      <c r="E7" s="188"/>
+      <c r="F7" s="188"/>
+      <c r="G7" s="188"/>
+      <c r="H7" s="188"/>
+      <c r="I7" s="188"/>
+      <c r="J7" s="188"/>
+      <c r="K7" s="188"/>
+      <c r="L7" s="188"/>
+      <c r="M7" s="189"/>
     </row>
     <row r="8" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="93" t="s">
+      <c r="A8" s="190" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="94"/>
-      <c r="C8" s="95"/>
-      <c r="D8" s="155"/>
-      <c r="E8" s="156"/>
-      <c r="F8" s="156"/>
-      <c r="G8" s="156"/>
-      <c r="H8" s="156"/>
-      <c r="I8" s="156"/>
-      <c r="J8" s="156"/>
-      <c r="K8" s="156"/>
-      <c r="L8" s="156"/>
-      <c r="M8" s="157"/>
+      <c r="B8" s="191"/>
+      <c r="C8" s="192"/>
+      <c r="D8" s="142"/>
+      <c r="E8" s="143"/>
+      <c r="F8" s="143"/>
+      <c r="G8" s="143"/>
+      <c r="H8" s="143"/>
+      <c r="I8" s="143"/>
+      <c r="J8" s="143"/>
+      <c r="K8" s="143"/>
+      <c r="L8" s="143"/>
+      <c r="M8" s="144"/>
     </row>
     <row r="9" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="84"/>
-      <c r="B9" s="85"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="158"/>
-      <c r="E9" s="159"/>
-      <c r="F9" s="159"/>
-      <c r="G9" s="159"/>
-      <c r="H9" s="159"/>
-      <c r="I9" s="159"/>
-      <c r="J9" s="159"/>
-      <c r="K9" s="159"/>
-      <c r="L9" s="159"/>
-      <c r="M9" s="160"/>
+      <c r="A9" s="181"/>
+      <c r="B9" s="182"/>
+      <c r="C9" s="183"/>
+      <c r="D9" s="145"/>
+      <c r="E9" s="146"/>
+      <c r="F9" s="146"/>
+      <c r="G9" s="146"/>
+      <c r="H9" s="146"/>
+      <c r="I9" s="146"/>
+      <c r="J9" s="146"/>
+      <c r="K9" s="146"/>
+      <c r="L9" s="146"/>
+      <c r="M9" s="147"/>
     </row>
     <row r="10" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="93" t="s">
+      <c r="A10" s="190" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="94"/>
-      <c r="C10" s="95"/>
-      <c r="D10" s="155"/>
-      <c r="E10" s="161"/>
-      <c r="F10" s="161"/>
-      <c r="G10" s="161"/>
-      <c r="H10" s="161"/>
-      <c r="I10" s="161"/>
-      <c r="J10" s="161"/>
-      <c r="K10" s="161"/>
-      <c r="L10" s="161"/>
-      <c r="M10" s="162"/>
+      <c r="B10" s="191"/>
+      <c r="C10" s="192"/>
+      <c r="D10" s="142"/>
+      <c r="E10" s="148"/>
+      <c r="F10" s="148"/>
+      <c r="G10" s="148"/>
+      <c r="H10" s="148"/>
+      <c r="I10" s="148"/>
+      <c r="J10" s="148"/>
+      <c r="K10" s="148"/>
+      <c r="L10" s="148"/>
+      <c r="M10" s="149"/>
     </row>
     <row r="11" spans="1:13" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="96"/>
-      <c r="B11" s="97"/>
-      <c r="C11" s="98"/>
-      <c r="D11" s="163"/>
-      <c r="E11" s="164"/>
-      <c r="F11" s="164"/>
-      <c r="G11" s="164"/>
-      <c r="H11" s="164"/>
-      <c r="I11" s="164"/>
-      <c r="J11" s="164"/>
-      <c r="K11" s="164"/>
-      <c r="L11" s="164"/>
-      <c r="M11" s="165"/>
+      <c r="A11" s="140"/>
+      <c r="B11" s="98"/>
+      <c r="C11" s="141"/>
+      <c r="D11" s="150"/>
+      <c r="E11" s="151"/>
+      <c r="F11" s="151"/>
+      <c r="G11" s="151"/>
+      <c r="H11" s="151"/>
+      <c r="I11" s="151"/>
+      <c r="J11" s="151"/>
+      <c r="K11" s="151"/>
+      <c r="L11" s="151"/>
+      <c r="M11" s="152"/>
     </row>
     <row r="12" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="137" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="82"/>
-      <c r="C12" s="83"/>
-      <c r="D12" s="120" t="s">
+      <c r="B12" s="138"/>
+      <c r="C12" s="139"/>
+      <c r="D12" s="165" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="124"/>
-      <c r="F12" s="124"/>
-      <c r="G12" s="124"/>
-      <c r="H12" s="125"/>
-      <c r="I12" s="129" t="s">
+      <c r="E12" s="167"/>
+      <c r="F12" s="167"/>
+      <c r="G12" s="167"/>
+      <c r="H12" s="168"/>
+      <c r="I12" s="172" t="s">
         <v>7</v>
       </c>
-      <c r="J12" s="130"/>
-      <c r="K12" s="133" t="s">
+      <c r="J12" s="173"/>
+      <c r="K12" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="L12" s="120" t="s">
+      <c r="L12" s="165" t="s">
         <v>9</v>
       </c>
-      <c r="M12" s="121"/>
+      <c r="M12" s="166"/>
     </row>
     <row r="13" spans="1:13" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="96"/>
-      <c r="B13" s="97"/>
-      <c r="C13" s="98"/>
-      <c r="D13" s="126"/>
-      <c r="E13" s="127"/>
-      <c r="F13" s="127"/>
-      <c r="G13" s="127"/>
-      <c r="H13" s="128"/>
-      <c r="I13" s="131"/>
-      <c r="J13" s="132"/>
-      <c r="K13" s="134"/>
-      <c r="L13" s="122"/>
-      <c r="M13" s="123"/>
+      <c r="A13" s="140"/>
+      <c r="B13" s="98"/>
+      <c r="C13" s="141"/>
+      <c r="D13" s="169"/>
+      <c r="E13" s="170"/>
+      <c r="F13" s="170"/>
+      <c r="G13" s="170"/>
+      <c r="H13" s="171"/>
+      <c r="I13" s="174"/>
+      <c r="J13" s="175"/>
+      <c r="K13" s="177"/>
+      <c r="L13" s="97"/>
+      <c r="M13" s="99"/>
     </row>
     <row r="14" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="143"/>
-      <c r="B14" s="119"/>
-      <c r="C14" s="113"/>
-      <c r="D14" s="112" t="s">
+      <c r="A14" s="116"/>
+      <c r="B14" s="117"/>
+      <c r="C14" s="118"/>
+      <c r="D14" s="119" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="119"/>
-      <c r="F14" s="119"/>
-      <c r="G14" s="119"/>
-      <c r="H14" s="113"/>
-      <c r="I14" s="112"/>
-      <c r="J14" s="113"/>
+      <c r="E14" s="117"/>
+      <c r="F14" s="117"/>
+      <c r="G14" s="117"/>
+      <c r="H14" s="118"/>
+      <c r="I14" s="119"/>
+      <c r="J14" s="118"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="114"/>
-      <c r="M14" s="115"/>
+      <c r="L14" s="120"/>
+      <c r="M14" s="121"/>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="143"/>
-      <c r="B15" s="119"/>
-      <c r="C15" s="113"/>
-      <c r="D15" s="152" t="s">
+      <c r="A15" s="116"/>
+      <c r="B15" s="117"/>
+      <c r="C15" s="118"/>
+      <c r="D15" s="134" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="153"/>
-      <c r="F15" s="153"/>
-      <c r="G15" s="153"/>
-      <c r="H15" s="154"/>
-      <c r="I15" s="112"/>
-      <c r="J15" s="113"/>
+      <c r="E15" s="135"/>
+      <c r="F15" s="135"/>
+      <c r="G15" s="135"/>
+      <c r="H15" s="136"/>
+      <c r="I15" s="119"/>
+      <c r="J15" s="118"/>
       <c r="K15" s="4"/>
-      <c r="L15" s="114"/>
-      <c r="M15" s="115"/>
+      <c r="L15" s="120"/>
+      <c r="M15" s="121"/>
     </row>
     <row r="16" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="143"/>
-      <c r="B16" s="119"/>
-      <c r="C16" s="113"/>
-      <c r="D16" s="152"/>
-      <c r="E16" s="153"/>
-      <c r="F16" s="153"/>
-      <c r="G16" s="153"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="112"/>
-      <c r="J16" s="113"/>
+      <c r="A16" s="116"/>
+      <c r="B16" s="117"/>
+      <c r="C16" s="118"/>
+      <c r="D16" s="134"/>
+      <c r="E16" s="135"/>
+      <c r="F16" s="135"/>
+      <c r="G16" s="135"/>
+      <c r="H16" s="136"/>
+      <c r="I16" s="119"/>
+      <c r="J16" s="118"/>
       <c r="K16" s="4"/>
-      <c r="L16" s="147" t="s">
+      <c r="L16" s="178" t="s">
         <v>47</v>
       </c>
-      <c r="M16" s="148"/>
+      <c r="M16" s="179"/>
     </row>
     <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="143"/>
-      <c r="B17" s="119"/>
-      <c r="C17" s="113"/>
-      <c r="D17" s="152"/>
-      <c r="E17" s="153"/>
-      <c r="F17" s="153"/>
-      <c r="G17" s="153"/>
-      <c r="H17" s="154"/>
-      <c r="I17" s="112"/>
-      <c r="J17" s="113"/>
+      <c r="A17" s="116"/>
+      <c r="B17" s="117"/>
+      <c r="C17" s="118"/>
+      <c r="D17" s="134"/>
+      <c r="E17" s="135"/>
+      <c r="F17" s="135"/>
+      <c r="G17" s="135"/>
+      <c r="H17" s="136"/>
+      <c r="I17" s="119"/>
+      <c r="J17" s="118"/>
       <c r="K17" s="4"/>
-      <c r="L17" s="114"/>
-      <c r="M17" s="115"/>
+      <c r="L17" s="120"/>
+      <c r="M17" s="121"/>
     </row>
     <row r="18" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="143"/>
-      <c r="B18" s="119"/>
-      <c r="C18" s="113"/>
-      <c r="D18" s="152"/>
-      <c r="E18" s="153"/>
-      <c r="F18" s="153"/>
-      <c r="G18" s="153"/>
-      <c r="H18" s="154"/>
-      <c r="I18" s="112"/>
-      <c r="J18" s="113"/>
+      <c r="A18" s="116"/>
+      <c r="B18" s="117"/>
+      <c r="C18" s="118"/>
+      <c r="D18" s="134"/>
+      <c r="E18" s="135"/>
+      <c r="F18" s="135"/>
+      <c r="G18" s="135"/>
+      <c r="H18" s="136"/>
+      <c r="I18" s="119"/>
+      <c r="J18" s="118"/>
       <c r="K18" s="4"/>
-      <c r="L18" s="114"/>
-      <c r="M18" s="115"/>
+      <c r="L18" s="120"/>
+      <c r="M18" s="121"/>
     </row>
     <row r="19" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="143"/>
-      <c r="B19" s="119"/>
-      <c r="C19" s="113"/>
-      <c r="D19" s="152"/>
-      <c r="E19" s="153"/>
-      <c r="F19" s="153"/>
-      <c r="G19" s="153"/>
-      <c r="H19" s="154"/>
-      <c r="I19" s="112"/>
-      <c r="J19" s="113"/>
+      <c r="A19" s="116"/>
+      <c r="B19" s="117"/>
+      <c r="C19" s="118"/>
+      <c r="D19" s="134"/>
+      <c r="E19" s="135"/>
+      <c r="F19" s="135"/>
+      <c r="G19" s="135"/>
+      <c r="H19" s="136"/>
+      <c r="I19" s="119"/>
+      <c r="J19" s="118"/>
       <c r="K19" s="4"/>
-      <c r="L19" s="114"/>
-      <c r="M19" s="115"/>
+      <c r="L19" s="120"/>
+      <c r="M19" s="121"/>
     </row>
     <row r="20" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="143"/>
-      <c r="B20" s="119"/>
-      <c r="C20" s="113"/>
-      <c r="D20" s="152"/>
-      <c r="E20" s="153"/>
-      <c r="F20" s="153"/>
-      <c r="G20" s="153"/>
-      <c r="H20" s="154"/>
-      <c r="I20" s="112"/>
-      <c r="J20" s="113"/>
+      <c r="A20" s="116"/>
+      <c r="B20" s="117"/>
+      <c r="C20" s="118"/>
+      <c r="D20" s="134"/>
+      <c r="E20" s="135"/>
+      <c r="F20" s="135"/>
+      <c r="G20" s="135"/>
+      <c r="H20" s="136"/>
+      <c r="I20" s="119"/>
+      <c r="J20" s="118"/>
       <c r="K20" s="4"/>
-      <c r="L20" s="114"/>
-      <c r="M20" s="115"/>
+      <c r="L20" s="120"/>
+      <c r="M20" s="121"/>
     </row>
     <row r="21" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="143"/>
-      <c r="B21" s="119"/>
-      <c r="C21" s="113"/>
+      <c r="A21" s="116"/>
+      <c r="B21" s="117"/>
+      <c r="C21" s="118"/>
       <c r="D21" s="5"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="7"/>
-      <c r="I21" s="112"/>
-      <c r="J21" s="113"/>
+      <c r="I21" s="119"/>
+      <c r="J21" s="118"/>
       <c r="K21" s="4"/>
-      <c r="L21" s="114"/>
-      <c r="M21" s="115"/>
+      <c r="L21" s="120"/>
+      <c r="M21" s="121"/>
     </row>
     <row r="22" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="143"/>
-      <c r="B22" s="119"/>
-      <c r="C22" s="113"/>
+      <c r="A22" s="116"/>
+      <c r="B22" s="117"/>
+      <c r="C22" s="118"/>
       <c r="D22" s="5"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="7"/>
-      <c r="I22" s="112"/>
-      <c r="J22" s="113"/>
+      <c r="I22" s="119"/>
+      <c r="J22" s="118"/>
       <c r="K22" s="4"/>
-      <c r="L22" s="114"/>
-      <c r="M22" s="115"/>
+      <c r="L22" s="120"/>
+      <c r="M22" s="121"/>
     </row>
     <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="143"/>
-      <c r="B23" s="119"/>
-      <c r="C23" s="113"/>
-      <c r="D23" s="144"/>
-      <c r="E23" s="145"/>
-      <c r="F23" s="145"/>
-      <c r="G23" s="145"/>
-      <c r="H23" s="146"/>
-      <c r="I23" s="112"/>
-      <c r="J23" s="113"/>
+      <c r="A23" s="116"/>
+      <c r="B23" s="117"/>
+      <c r="C23" s="118"/>
+      <c r="D23" s="153"/>
+      <c r="E23" s="110"/>
+      <c r="F23" s="110"/>
+      <c r="G23" s="110"/>
+      <c r="H23" s="154"/>
+      <c r="I23" s="119"/>
+      <c r="J23" s="118"/>
       <c r="K23" s="4"/>
-      <c r="L23" s="114"/>
-      <c r="M23" s="115"/>
+      <c r="L23" s="120"/>
+      <c r="M23" s="121"/>
     </row>
     <row r="24" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="143"/>
-      <c r="B24" s="119"/>
-      <c r="C24" s="113"/>
-      <c r="D24" s="144"/>
-      <c r="E24" s="145"/>
-      <c r="F24" s="145"/>
-      <c r="G24" s="145"/>
-      <c r="H24" s="146"/>
-      <c r="I24" s="112"/>
-      <c r="J24" s="113"/>
+      <c r="A24" s="116"/>
+      <c r="B24" s="117"/>
+      <c r="C24" s="118"/>
+      <c r="D24" s="153"/>
+      <c r="E24" s="110"/>
+      <c r="F24" s="110"/>
+      <c r="G24" s="110"/>
+      <c r="H24" s="154"/>
+      <c r="I24" s="119"/>
+      <c r="J24" s="118"/>
       <c r="K24" s="4"/>
-      <c r="L24" s="114"/>
-      <c r="M24" s="115"/>
+      <c r="L24" s="120"/>
+      <c r="M24" s="121"/>
     </row>
     <row r="25" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="143"/>
-      <c r="B25" s="119"/>
-      <c r="C25" s="113"/>
-      <c r="D25" s="144"/>
-      <c r="E25" s="145"/>
-      <c r="F25" s="145"/>
-      <c r="G25" s="145"/>
-      <c r="H25" s="146"/>
-      <c r="I25" s="112"/>
-      <c r="J25" s="113"/>
+      <c r="A25" s="116"/>
+      <c r="B25" s="117"/>
+      <c r="C25" s="118"/>
+      <c r="D25" s="153"/>
+      <c r="E25" s="110"/>
+      <c r="F25" s="110"/>
+      <c r="G25" s="110"/>
+      <c r="H25" s="154"/>
+      <c r="I25" s="119"/>
+      <c r="J25" s="118"/>
       <c r="K25" s="4"/>
-      <c r="L25" s="114"/>
-      <c r="M25" s="115"/>
+      <c r="L25" s="120"/>
+      <c r="M25" s="121"/>
     </row>
     <row r="26" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="143"/>
-      <c r="B26" s="119"/>
-      <c r="C26" s="113"/>
-      <c r="D26" s="112"/>
-      <c r="E26" s="119"/>
-      <c r="F26" s="119"/>
-      <c r="G26" s="119"/>
-      <c r="H26" s="113"/>
-      <c r="I26" s="112"/>
-      <c r="J26" s="113"/>
+      <c r="A26" s="116"/>
+      <c r="B26" s="117"/>
+      <c r="C26" s="118"/>
+      <c r="D26" s="119"/>
+      <c r="E26" s="117"/>
+      <c r="F26" s="117"/>
+      <c r="G26" s="117"/>
+      <c r="H26" s="118"/>
+      <c r="I26" s="119"/>
+      <c r="J26" s="118"/>
       <c r="K26" s="4"/>
-      <c r="L26" s="114"/>
-      <c r="M26" s="115"/>
+      <c r="L26" s="120"/>
+      <c r="M26" s="121"/>
     </row>
     <row r="27" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="143"/>
-      <c r="B27" s="119"/>
-      <c r="C27" s="113"/>
-      <c r="D27" s="112"/>
-      <c r="E27" s="119"/>
-      <c r="F27" s="119"/>
-      <c r="G27" s="119"/>
-      <c r="H27" s="113"/>
-      <c r="I27" s="112"/>
-      <c r="J27" s="113"/>
+      <c r="A27" s="116"/>
+      <c r="B27" s="117"/>
+      <c r="C27" s="118"/>
+      <c r="D27" s="119"/>
+      <c r="E27" s="117"/>
+      <c r="F27" s="117"/>
+      <c r="G27" s="117"/>
+      <c r="H27" s="118"/>
+      <c r="I27" s="119"/>
+      <c r="J27" s="118"/>
       <c r="K27" s="8"/>
-      <c r="L27" s="114"/>
-      <c r="M27" s="115"/>
+      <c r="L27" s="120"/>
+      <c r="M27" s="121"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="143"/>
-      <c r="B28" s="119"/>
-      <c r="C28" s="113"/>
-      <c r="D28" s="112"/>
-      <c r="E28" s="119"/>
-      <c r="F28" s="119"/>
-      <c r="G28" s="119"/>
-      <c r="H28" s="113"/>
-      <c r="I28" s="112"/>
-      <c r="J28" s="113"/>
+      <c r="A28" s="116"/>
+      <c r="B28" s="117"/>
+      <c r="C28" s="118"/>
+      <c r="D28" s="119"/>
+      <c r="E28" s="117"/>
+      <c r="F28" s="117"/>
+      <c r="G28" s="117"/>
+      <c r="H28" s="118"/>
+      <c r="I28" s="119"/>
+      <c r="J28" s="118"/>
       <c r="K28" s="8"/>
-      <c r="L28" s="114"/>
-      <c r="M28" s="115"/>
+      <c r="L28" s="120"/>
+      <c r="M28" s="121"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="143"/>
-      <c r="B29" s="119"/>
-      <c r="C29" s="113"/>
-      <c r="D29" s="112"/>
-      <c r="E29" s="119"/>
-      <c r="F29" s="119"/>
-      <c r="G29" s="119"/>
-      <c r="H29" s="113"/>
-      <c r="I29" s="112"/>
-      <c r="J29" s="113"/>
+      <c r="A29" s="116"/>
+      <c r="B29" s="117"/>
+      <c r="C29" s="118"/>
+      <c r="D29" s="119"/>
+      <c r="E29" s="117"/>
+      <c r="F29" s="117"/>
+      <c r="G29" s="117"/>
+      <c r="H29" s="118"/>
+      <c r="I29" s="119"/>
+      <c r="J29" s="118"/>
       <c r="K29" s="8"/>
-      <c r="L29" s="114"/>
-      <c r="M29" s="115"/>
+      <c r="L29" s="120"/>
+      <c r="M29" s="121"/>
     </row>
     <row r="30" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="143"/>
-      <c r="B30" s="119"/>
-      <c r="C30" s="113"/>
-      <c r="D30" s="112"/>
-      <c r="E30" s="119"/>
-      <c r="F30" s="119"/>
-      <c r="G30" s="119"/>
-      <c r="H30" s="113"/>
-      <c r="I30" s="112"/>
-      <c r="J30" s="113"/>
+      <c r="A30" s="116"/>
+      <c r="B30" s="117"/>
+      <c r="C30" s="118"/>
+      <c r="D30" s="119"/>
+      <c r="E30" s="117"/>
+      <c r="F30" s="117"/>
+      <c r="G30" s="117"/>
+      <c r="H30" s="118"/>
+      <c r="I30" s="119"/>
+      <c r="J30" s="118"/>
       <c r="K30" s="8"/>
-      <c r="L30" s="114"/>
-      <c r="M30" s="115"/>
+      <c r="L30" s="120"/>
+      <c r="M30" s="121"/>
     </row>
     <row r="31" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="143"/>
-      <c r="B31" s="119"/>
-      <c r="C31" s="113"/>
-      <c r="D31" s="112"/>
-      <c r="E31" s="119"/>
-      <c r="F31" s="119"/>
-      <c r="G31" s="119"/>
-      <c r="H31" s="113"/>
-      <c r="I31" s="112"/>
-      <c r="J31" s="113"/>
+      <c r="A31" s="116"/>
+      <c r="B31" s="117"/>
+      <c r="C31" s="118"/>
+      <c r="D31" s="119"/>
+      <c r="E31" s="117"/>
+      <c r="F31" s="117"/>
+      <c r="G31" s="117"/>
+      <c r="H31" s="118"/>
+      <c r="I31" s="119"/>
+      <c r="J31" s="118"/>
       <c r="K31" s="8"/>
-      <c r="L31" s="114"/>
-      <c r="M31" s="115"/>
+      <c r="L31" s="120"/>
+      <c r="M31" s="121"/>
     </row>
     <row r="32" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="143"/>
-      <c r="B32" s="119"/>
-      <c r="C32" s="113"/>
-      <c r="D32" s="112"/>
-      <c r="E32" s="119"/>
-      <c r="F32" s="119"/>
-      <c r="G32" s="119"/>
-      <c r="H32" s="113"/>
-      <c r="I32" s="112"/>
-      <c r="J32" s="113"/>
+      <c r="A32" s="116"/>
+      <c r="B32" s="117"/>
+      <c r="C32" s="118"/>
+      <c r="D32" s="119"/>
+      <c r="E32" s="117"/>
+      <c r="F32" s="117"/>
+      <c r="G32" s="117"/>
+      <c r="H32" s="118"/>
+      <c r="I32" s="119"/>
+      <c r="J32" s="118"/>
       <c r="K32" s="8"/>
-      <c r="L32" s="114"/>
-      <c r="M32" s="115"/>
+      <c r="L32" s="120"/>
+      <c r="M32" s="121"/>
     </row>
     <row r="33" spans="1:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="166"/>
-      <c r="B33" s="167"/>
-      <c r="C33" s="168"/>
-      <c r="D33" s="169" t="s">
+      <c r="A33" s="122"/>
+      <c r="B33" s="123"/>
+      <c r="C33" s="124"/>
+      <c r="D33" s="125" t="s">
         <v>11</v>
       </c>
-      <c r="E33" s="170"/>
-      <c r="F33" s="170"/>
-      <c r="G33" s="170"/>
-      <c r="H33" s="171"/>
-      <c r="I33" s="172"/>
-      <c r="J33" s="168"/>
+      <c r="E33" s="126"/>
+      <c r="F33" s="126"/>
+      <c r="G33" s="126"/>
+      <c r="H33" s="127"/>
+      <c r="I33" s="128"/>
+      <c r="J33" s="124"/>
       <c r="K33" s="9"/>
-      <c r="L33" s="173" t="str">
+      <c r="L33" s="129" t="str">
         <f>L16</f>
         <v>6,000.00</v>
       </c>
-      <c r="M33" s="174"/>
+      <c r="M33" s="130"/>
     </row>
     <row r="34" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="135" t="s">
+      <c r="A34" s="155" t="s">
         <v>12</v>
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="11"/>
-      <c r="D34" s="137" t="s">
+      <c r="D34" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="E34" s="138"/>
-      <c r="F34" s="138"/>
-      <c r="G34" s="138"/>
-      <c r="H34" s="139"/>
-      <c r="I34" s="140" t="s">
+      <c r="E34" s="157"/>
+      <c r="F34" s="157"/>
+      <c r="G34" s="157"/>
+      <c r="H34" s="158"/>
+      <c r="I34" s="159" t="s">
         <v>14</v>
       </c>
       <c r="J34" s="12"/>
@@ -3216,17 +3225,17 @@
       <c r="M34" s="13"/>
     </row>
     <row r="35" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="136"/>
-      <c r="B35" s="141" t="s">
+      <c r="A35" s="156"/>
+      <c r="B35" s="160" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="142"/>
-      <c r="D35" s="138"/>
-      <c r="E35" s="138"/>
-      <c r="F35" s="138"/>
-      <c r="G35" s="138"/>
-      <c r="H35" s="139"/>
-      <c r="I35" s="140"/>
+      <c r="C35" s="161"/>
+      <c r="D35" s="157"/>
+      <c r="E35" s="157"/>
+      <c r="F35" s="157"/>
+      <c r="G35" s="157"/>
+      <c r="H35" s="158"/>
+      <c r="I35" s="159"/>
       <c r="J35" s="14" t="s">
         <v>48</v>
       </c>
@@ -3236,15 +3245,15 @@
     </row>
     <row r="36" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
-      <c r="B36" s="145" t="s">
+      <c r="B36" s="110" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="145"/>
-      <c r="D36" s="145"/>
-      <c r="E36" s="145"/>
-      <c r="F36" s="145"/>
-      <c r="G36" s="145"/>
-      <c r="H36" s="184"/>
+      <c r="C36" s="110"/>
+      <c r="D36" s="110"/>
+      <c r="E36" s="110"/>
+      <c r="F36" s="110"/>
+      <c r="G36" s="110"/>
+      <c r="H36" s="111"/>
       <c r="I36" s="16"/>
       <c r="J36" s="11" t="s">
         <v>17</v>
@@ -3254,7 +3263,7 @@
       <c r="M36" s="13"/>
     </row>
     <row r="37" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="185"/>
+      <c r="A37" s="112"/>
       <c r="B37" s="11" t="s">
         <v>18</v>
       </c>
@@ -3273,7 +3282,7 @@
       <c r="M37" s="13"/>
     </row>
     <row r="38" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="185"/>
+      <c r="A38" s="112"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
@@ -3322,14 +3331,14 @@
         <v>21</v>
       </c>
       <c r="B41" s="11"/>
-      <c r="C41" s="186" t="s">
+      <c r="C41" s="113" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="186"/>
-      <c r="E41" s="186"/>
-      <c r="F41" s="186"/>
-      <c r="G41" s="186"/>
-      <c r="H41" s="187"/>
+      <c r="D41" s="113"/>
+      <c r="E41" s="113"/>
+      <c r="F41" s="113"/>
+      <c r="G41" s="113"/>
+      <c r="H41" s="114"/>
       <c r="I41" s="11" t="s">
         <v>21</v>
       </c>
@@ -3394,18 +3403,18 @@
       <c r="M44" s="13"/>
     </row>
     <row r="45" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="177" t="s">
+      <c r="A45" s="104" t="s">
         <v>25</v>
       </c>
-      <c r="B45" s="178"/>
-      <c r="C45" s="188" t="s">
+      <c r="B45" s="105"/>
+      <c r="C45" s="115" t="s">
         <v>50</v>
       </c>
-      <c r="D45" s="137"/>
-      <c r="E45" s="137"/>
-      <c r="F45" s="137"/>
-      <c r="G45" s="137"/>
-      <c r="H45" s="179"/>
+      <c r="D45" s="86"/>
+      <c r="E45" s="86"/>
+      <c r="F45" s="86"/>
+      <c r="G45" s="86"/>
+      <c r="H45" s="87"/>
       <c r="I45" s="11" t="s">
         <v>25</v>
       </c>
@@ -3419,12 +3428,12 @@
     <row r="46" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="26"/>
       <c r="B46" s="27"/>
-      <c r="C46" s="175"/>
-      <c r="D46" s="175"/>
-      <c r="E46" s="175"/>
-      <c r="F46" s="175"/>
-      <c r="G46" s="175"/>
-      <c r="H46" s="176"/>
+      <c r="C46" s="102"/>
+      <c r="D46" s="102"/>
+      <c r="E46" s="102"/>
+      <c r="F46" s="102"/>
+      <c r="G46" s="102"/>
+      <c r="H46" s="103"/>
       <c r="I46" s="11"/>
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
@@ -3432,18 +3441,18 @@
       <c r="M46" s="13"/>
     </row>
     <row r="47" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="177" t="s">
+      <c r="A47" s="104" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="178"/>
-      <c r="C47" s="137" t="s">
+      <c r="B47" s="105"/>
+      <c r="C47" s="86" t="s">
         <v>20</v>
       </c>
-      <c r="D47" s="137"/>
-      <c r="E47" s="137"/>
-      <c r="F47" s="137"/>
-      <c r="G47" s="137"/>
-      <c r="H47" s="179"/>
+      <c r="D47" s="86"/>
+      <c r="E47" s="86"/>
+      <c r="F47" s="86"/>
+      <c r="G47" s="86"/>
+      <c r="H47" s="87"/>
       <c r="I47" s="11" t="s">
         <v>26</v>
       </c>
@@ -3488,81 +3497,81 @@
       <c r="A50" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="B50" s="180" t="s">
+      <c r="B50" s="106" t="s">
         <v>28</v>
       </c>
-      <c r="C50" s="181"/>
-      <c r="D50" s="181"/>
-      <c r="E50" s="181"/>
-      <c r="F50" s="181"/>
-      <c r="G50" s="181"/>
-      <c r="H50" s="181"/>
-      <c r="I50" s="181"/>
-      <c r="J50" s="181"/>
-      <c r="K50" s="181"/>
-      <c r="L50" s="181"/>
-      <c r="M50" s="182"/>
+      <c r="C50" s="107"/>
+      <c r="D50" s="107"/>
+      <c r="E50" s="107"/>
+      <c r="F50" s="107"/>
+      <c r="G50" s="107"/>
+      <c r="H50" s="107"/>
+      <c r="I50" s="107"/>
+      <c r="J50" s="107"/>
+      <c r="K50" s="107"/>
+      <c r="L50" s="107"/>
+      <c r="M50" s="108"/>
     </row>
     <row r="51" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="183" t="s">
+      <c r="A51" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="B51" s="181"/>
-      <c r="C51" s="181"/>
-      <c r="D51" s="181"/>
-      <c r="E51" s="181"/>
-      <c r="F51" s="181"/>
-      <c r="G51" s="182"/>
-      <c r="H51" s="183" t="s">
+      <c r="B51" s="107"/>
+      <c r="C51" s="107"/>
+      <c r="D51" s="107"/>
+      <c r="E51" s="107"/>
+      <c r="F51" s="107"/>
+      <c r="G51" s="108"/>
+      <c r="H51" s="109" t="s">
         <v>9</v>
       </c>
-      <c r="I51" s="181"/>
-      <c r="J51" s="181"/>
-      <c r="K51" s="181"/>
-      <c r="L51" s="181"/>
-      <c r="M51" s="182"/>
+      <c r="I51" s="107"/>
+      <c r="J51" s="107"/>
+      <c r="K51" s="107"/>
+      <c r="L51" s="107"/>
+      <c r="M51" s="108"/>
     </row>
     <row r="52" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="195" t="s">
+      <c r="A52" s="88" t="s">
         <v>30</v>
       </c>
-      <c r="B52" s="197" t="s">
+      <c r="B52" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="C52" s="198"/>
-      <c r="D52" s="198"/>
-      <c r="E52" s="201" t="s">
+      <c r="C52" s="91"/>
+      <c r="D52" s="91"/>
+      <c r="E52" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="F52" s="202"/>
-      <c r="G52" s="203"/>
-      <c r="H52" s="195" t="s">
+      <c r="F52" s="95"/>
+      <c r="G52" s="96"/>
+      <c r="H52" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="I52" s="204" t="s">
+      <c r="I52" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="J52" s="205"/>
-      <c r="K52" s="189" t="s">
+      <c r="J52" s="101"/>
+      <c r="K52" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="L52" s="190" t="s">
+      <c r="L52" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="M52" s="191"/>
+      <c r="M52" s="82"/>
     </row>
     <row r="53" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="195"/>
-      <c r="B53" s="197"/>
-      <c r="C53" s="198"/>
-      <c r="D53" s="198"/>
-      <c r="E53" s="201"/>
-      <c r="F53" s="202"/>
-      <c r="G53" s="203"/>
-      <c r="H53" s="195"/>
-      <c r="I53" s="204"/>
-      <c r="J53" s="205"/>
-      <c r="K53" s="189"/>
+      <c r="A53" s="88"/>
+      <c r="B53" s="90"/>
+      <c r="C53" s="91"/>
+      <c r="D53" s="91"/>
+      <c r="E53" s="94"/>
+      <c r="F53" s="95"/>
+      <c r="G53" s="96"/>
+      <c r="H53" s="88"/>
+      <c r="I53" s="100"/>
+      <c r="J53" s="101"/>
+      <c r="K53" s="80"/>
       <c r="L53" s="38" t="s">
         <v>35</v>
       </c>
@@ -3571,20 +3580,20 @@
       </c>
     </row>
     <row r="54" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="196"/>
-      <c r="B54" s="199"/>
-      <c r="C54" s="200"/>
-      <c r="D54" s="200"/>
-      <c r="E54" s="122"/>
-      <c r="F54" s="97"/>
-      <c r="G54" s="123"/>
+      <c r="A54" s="89"/>
+      <c r="B54" s="92"/>
+      <c r="C54" s="93"/>
+      <c r="D54" s="93"/>
+      <c r="E54" s="97"/>
+      <c r="F54" s="98"/>
+      <c r="G54" s="99"/>
       <c r="H54" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="I54" s="192" t="s">
+      <c r="I54" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="J54" s="193"/>
+      <c r="J54" s="84"/>
       <c r="K54" s="41" t="s">
         <v>39</v>
       </c>
@@ -3608,9 +3617,9 @@
     </row>
     <row r="56" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="44"/>
-      <c r="B56" s="45"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="46"/>
+      <c r="B56" s="206"/>
+      <c r="C56" s="207"/>
+      <c r="D56" s="208"/>
       <c r="E56" s="47"/>
       <c r="F56" s="17"/>
       <c r="G56" s="48"/>
@@ -3623,9 +3632,9 @@
     </row>
     <row r="57" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="44"/>
-      <c r="B57" s="45"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="46"/>
+      <c r="B57" s="206"/>
+      <c r="C57" s="207"/>
+      <c r="D57" s="208"/>
       <c r="E57" s="55"/>
       <c r="F57" s="17"/>
       <c r="G57" s="48"/>
@@ -3638,12 +3647,12 @@
     </row>
     <row r="58" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="44"/>
-      <c r="B58" s="45"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="46"/>
-      <c r="E58" s="194"/>
-      <c r="F58" s="137"/>
-      <c r="G58" s="179"/>
+      <c r="B58" s="206"/>
+      <c r="C58" s="207"/>
+      <c r="D58" s="208"/>
+      <c r="E58" s="85"/>
+      <c r="F58" s="86"/>
+      <c r="G58" s="87"/>
       <c r="H58" s="49"/>
       <c r="I58" s="50"/>
       <c r="J58" s="56"/>
@@ -3653,9 +3662,9 @@
     </row>
     <row r="59" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="44"/>
-      <c r="B59" s="45"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="46"/>
+      <c r="B59" s="206"/>
+      <c r="C59" s="207"/>
+      <c r="D59" s="208"/>
       <c r="E59" s="55"/>
       <c r="F59" s="17"/>
       <c r="G59" s="48"/>
@@ -3668,9 +3677,9 @@
     </row>
     <row r="60" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="44"/>
-      <c r="B60" s="45"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="46"/>
+      <c r="B60" s="206"/>
+      <c r="C60" s="207"/>
+      <c r="D60" s="208"/>
       <c r="E60" s="60"/>
       <c r="F60" s="17"/>
       <c r="G60" s="48"/>
@@ -3683,9 +3692,9 @@
     </row>
     <row r="61" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="44"/>
-      <c r="B61" s="45"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="46"/>
+      <c r="B61" s="206"/>
+      <c r="C61" s="207"/>
+      <c r="D61" s="208"/>
       <c r="E61" s="60"/>
       <c r="F61" s="17"/>
       <c r="G61" s="48"/>
@@ -3698,9 +3707,9 @@
     </row>
     <row r="62" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="44"/>
-      <c r="B62" s="45"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="46"/>
+      <c r="B62" s="206"/>
+      <c r="C62" s="207"/>
+      <c r="D62" s="208"/>
       <c r="E62" s="60"/>
       <c r="F62" s="17"/>
       <c r="G62" s="48"/>
@@ -3728,74 +3737,29 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="116">
-    <mergeCell ref="K52:K53"/>
-    <mergeCell ref="L52:M52"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="B52:D54"/>
-    <mergeCell ref="E52:G54"/>
-    <mergeCell ref="H52:H53"/>
-    <mergeCell ref="I52:J53"/>
-    <mergeCell ref="C46:H46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:H47"/>
-    <mergeCell ref="B50:M50"/>
-    <mergeCell ref="A51:G51"/>
-    <mergeCell ref="H51:M51"/>
-    <mergeCell ref="B36:H36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="C41:H41"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="C45:H45"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="D32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="D33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="D30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="D31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="D15:H20"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="A12:C13"/>
-    <mergeCell ref="D8:M9"/>
-    <mergeCell ref="D10:M11"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="D23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="D24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="L24:M24"/>
+  <mergeCells count="117">
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="A6:C7"/>
+    <mergeCell ref="D6:M7"/>
+    <mergeCell ref="A8:C9"/>
+    <mergeCell ref="A10:C11"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="D14:H14"/>
+    <mergeCell ref="L12:M13"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="D12:H13"/>
+    <mergeCell ref="I12:J13"/>
+    <mergeCell ref="K12:K13"/>
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="D34:H35"/>
     <mergeCell ref="I34:I35"/>
@@ -3820,34 +3784,80 @@
     <mergeCell ref="D27:H27"/>
     <mergeCell ref="I27:J27"/>
     <mergeCell ref="L27:M27"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="D15:H20"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="A12:C13"/>
+    <mergeCell ref="D8:M9"/>
+    <mergeCell ref="D10:M11"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="I17:J17"/>
     <mergeCell ref="I18:J18"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="L15:M15"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="D14:H14"/>
-    <mergeCell ref="L12:M13"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="D12:H13"/>
-    <mergeCell ref="I12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="A6:C7"/>
-    <mergeCell ref="D6:M7"/>
-    <mergeCell ref="A8:C9"/>
-    <mergeCell ref="A10:C11"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="D32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="D33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="D30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="D31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="C46:H46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:H47"/>
+    <mergeCell ref="B50:M50"/>
+    <mergeCell ref="A51:G51"/>
+    <mergeCell ref="H51:M51"/>
+    <mergeCell ref="B36:H36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="C41:H41"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="C45:H45"/>
+    <mergeCell ref="K52:K53"/>
+    <mergeCell ref="L52:M52"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="B52:D54"/>
+    <mergeCell ref="E52:G54"/>
+    <mergeCell ref="H52:H53"/>
+    <mergeCell ref="I52:J53"/>
+    <mergeCell ref="B56:D62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="78" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="77" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>